<commit_message>
more or less safe remark upload
</commit_message>
<xml_diff>
--- a/public/templates/remarks_template.xlsx
+++ b/public/templates/remarks_template.xlsx
@@ -11,87 +11,73 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="location_type">Лист2!$B$2:$B$4</definedName>
+    <definedName name="remark_level">Лист2!$D$2:$D$4</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>artifact</t>
-  </si>
-  <si>
-    <t>remark</t>
-  </si>
-  <si>
-    <t>type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+  <si>
+    <t>major</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>remark_level</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>diagram</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>line_number</t>
+  </si>
+  <si>
+    <t>element_number</t>
+  </si>
+  <si>
+    <t>element_name</t>
+  </si>
+  <si>
+    <t>element_type</t>
+  </si>
+  <si>
+    <t>location_type</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
   <si>
     <t>s-number</t>
-  </si>
-  <si>
-    <t>major</t>
-  </si>
-  <si>
-    <t>fake_file_name</t>
-  </si>
-  <si>
-    <t>fake_number</t>
-  </si>
-  <si>
-    <t>here you are fake remark</t>
-  </si>
-  <si>
-    <t>does not exist</t>
-  </si>
-  <si>
-    <t>outer space</t>
-  </si>
-  <si>
-    <t>line 2</t>
-  </si>
-  <si>
-    <t>artifact 1</t>
-  </si>
-  <si>
-    <t>seems that you have a problem with thesis</t>
-  </si>
-  <si>
-    <t>diagram 1</t>
-  </si>
-  <si>
-    <t>minor</t>
-  </si>
-  <si>
-    <t>s072435</t>
-  </si>
-  <si>
-    <t>diagram 2</t>
-  </si>
-  <si>
-    <t>Where is the fucking class diagram?</t>
-  </si>
-  <si>
-    <t>I didn't find your database organization structure diagram?</t>
-  </si>
-  <si>
-    <t>inspection</t>
-  </si>
-  <si>
-    <t>The FIT tool SUCKS!!!!</t>
-  </si>
-  <si>
-    <t>s082941</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +94,8 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,7 +104,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,8 +124,49 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -149,53 +174,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -205,19 +189,55 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,144 +534,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" customWidth="1"/>
-    <col min="6" max="9" width="46.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E17:E22">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>EXACT(C17,"code")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F12">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>EXACT(B2,"code")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:D12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>OR(EXACT($B2,"document"),EXACT($B2,"model"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:H12">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>EXACT($B2,"model")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E12">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>EXACT($B2,"document")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations xWindow="1181" yWindow="238" count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select location type from list" prompt="Click dropdown to select the value" sqref="B2:B12">
+      <formula1>location_type</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12">
+      <formula1>0</formula1>
+      <formula2>100000000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select remark level" prompt="Choose remark level from dropdown menu" sqref="J2:J12">
+      <formula1>remark_level</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -659,13 +798,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>